<commit_message>
Added 12765 and 12785 surrogates
</commit_message>
<xml_diff>
--- a/data/Compound_Descriptions/dryer_surr.xlsx
+++ b/data/Compound_Descriptions/dryer_surr.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="180" windowWidth="30740" windowHeight="16480"/>
+    <workbookView xWindow="3940" yWindow="2680" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,8 +447,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -458,11 +460,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -796,7 +800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1171,13 +1175,13 @@
     </row>
     <row r="2" spans="1:122" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -1204,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -1213,7 +1217,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -1450,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="CP2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CQ2" s="1">
         <v>0</v>
@@ -1539,16 +1543,16 @@
     </row>
     <row r="3" spans="1:122" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -1776,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="CB3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC3" s="1">
         <v>0</v>
@@ -1907,16 +1911,16 @@
     </row>
     <row r="4" spans="1:122" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -1940,13 +1944,13 @@
         <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O4" s="1">
         <v>0</v>
@@ -2144,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="CB4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC4" s="1">
         <v>0</v>
@@ -2275,13 +2279,13 @@
     </row>
     <row r="5" spans="1:122" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -2308,16 +2312,16 @@
         <v>0</v>
       </c>
       <c r="L5" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
@@ -2554,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="CP5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CQ5" s="1">
         <v>0</v>

</xml_diff>